<commit_message>
updated with latest occurrence data
</commit_message>
<xml_diff>
--- a/output/sites.xlsx
+++ b/output/sites.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
-  <si>
-    <t>full_name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+  <si>
+    <t>name</t>
   </si>
   <si>
     <t>records</t>
@@ -176,9 +176,6 @@
     <t>47</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>Aldabra Atoll</t>
   </si>
   <si>
@@ -203,12 +200,6 @@
     <t>Coiba National Park and its Special Zone of Marine Protection</t>
   </si>
   <si>
-    <t>Danube Delta</t>
-  </si>
-  <si>
-    <t>Desembarco del Granma National Park</t>
-  </si>
-  <si>
     <t>East Rennell</t>
   </si>
   <si>
@@ -221,9 +212,6 @@
     <t>Galápagos Islands</t>
   </si>
   <si>
-    <t>Giant's Causeway and Causeway Coast</t>
-  </si>
-  <si>
     <t>Gough and Inaccessible Islands</t>
   </si>
   <si>
@@ -239,9 +227,6 @@
     <t>Heard and McDonald Islands</t>
   </si>
   <si>
-    <t>Henderson Island</t>
-  </si>
-  <si>
     <t>High Coast / Kvarken Archipelago</t>
   </si>
   <si>
@@ -251,6 +236,12 @@
     <t>iSimangaliso Wetland Park</t>
   </si>
   <si>
+    <t>Islands and Protected Areas of the Gulf of California</t>
+  </si>
+  <si>
+    <t>Kluane / Wrangell-St Elias / Glacier Bay / Tatshenshini-Alsek</t>
+  </si>
+  <si>
     <t>Komodo National Park</t>
   </si>
   <si>
@@ -266,9 +257,6 @@
     <t>Malpelo Fauna and Flora Sanctuary</t>
   </si>
   <si>
-    <t>Mistaken Point</t>
-  </si>
-  <si>
     <t>Natural System of Wrangel Island Reserve</t>
   </si>
   <si>
@@ -284,12 +272,12 @@
     <t>Papahānaumokuākea</t>
   </si>
   <si>
+    <t>Pen?nsula Vald?s</t>
+  </si>
+  <si>
     <t>Phoenix Islands Protected Area</t>
   </si>
   <si>
-    <t>Pitons Management Area</t>
-  </si>
-  <si>
     <t>Rock Islands Southern Lagoon</t>
   </si>
   <si>
@@ -302,6 +290,9 @@
     <t>Shiretoko</t>
   </si>
   <si>
+    <t>Sian Ka'an</t>
+  </si>
+  <si>
     <t>Socotra Archipelago</t>
   </si>
   <si>
@@ -320,7 +311,10 @@
     <t>Ujung Kulon National Park</t>
   </si>
   <si>
-    <t>Vallée de Mai Nature Reserve</t>
+    <t>West Norwegian Fjords – Geirangerfjord and Nærøyfjord</t>
+  </si>
+  <si>
+    <t>Whale Sanctuary of El Vizcaino</t>
   </si>
 </sst>
 </file>
@@ -400,25 +394,25 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="n">
-        <v>801.0</v>
+        <v>3188.0</v>
       </c>
       <c r="D2" t="n">
-        <v>265.0</v>
+        <v>1041.0</v>
       </c>
       <c r="E2" t="n">
-        <v>231.0</v>
+        <v>501.0</v>
       </c>
       <c r="F2" t="n">
-        <v>6.0</v>
+        <v>65.0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="H2" t="n">
-        <v>219.0</v>
+        <v>456.0</v>
       </c>
     </row>
     <row r="3">
@@ -426,25 +420,25 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="n">
-        <v>7142.0</v>
+        <v>7435.0</v>
       </c>
       <c r="D3" t="n">
-        <v>433.0</v>
+        <v>464.0</v>
       </c>
       <c r="E3" t="n">
-        <v>367.0</v>
+        <v>379.0</v>
       </c>
       <c r="F3" t="n">
-        <v>50.0</v>
+        <v>61.0</v>
       </c>
       <c r="G3" t="n">
-        <v>46.0</v>
+        <v>49.0</v>
       </c>
       <c r="H3" t="n">
-        <v>283.0</v>
+        <v>294.0</v>
       </c>
     </row>
     <row r="4">
@@ -452,16 +446,16 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="n">
-        <v>1130.0</v>
+        <v>1102.0</v>
       </c>
       <c r="D4" t="n">
-        <v>366.0</v>
+        <v>354.0</v>
       </c>
       <c r="E4" t="n">
-        <v>359.0</v>
+        <v>347.0</v>
       </c>
       <c r="F4" t="n">
         <v>15.0</v>
@@ -470,7 +464,7 @@
         <v>12.0</v>
       </c>
       <c r="H4" t="n">
-        <v>242.0</v>
+        <v>230.0</v>
       </c>
     </row>
     <row r="5">
@@ -478,7 +472,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="n">
         <v>113.0</v>
@@ -504,13 +498,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="n">
-        <v>7995.0</v>
+        <v>8005.0</v>
       </c>
       <c r="D6" t="n">
-        <v>1077.0</v>
+        <v>1078.0</v>
       </c>
       <c r="E6" t="n">
         <v>349.0</v>
@@ -530,25 +524,25 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="n">
-        <v>349.0</v>
+        <v>26500.0</v>
       </c>
       <c r="D7" t="n">
-        <v>116.0</v>
+        <v>520.0</v>
       </c>
       <c r="E7" t="n">
-        <v>62.0</v>
+        <v>168.0</v>
       </c>
       <c r="F7" t="n">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
       <c r="G7" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="H7" t="n">
-        <v>58.0</v>
+        <v>147.0</v>
       </c>
     </row>
     <row r="8">
@@ -556,13 +550,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>2301.0</v>
+        <v>2304.0</v>
       </c>
       <c r="D8" t="n">
-        <v>492.0</v>
+        <v>494.0</v>
       </c>
       <c r="E8" t="n">
         <v>410.0</v>
@@ -582,16 +576,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="n">
-        <v>2329.0</v>
+        <v>2379.0</v>
       </c>
       <c r="D9" t="n">
-        <v>488.0</v>
+        <v>490.0</v>
       </c>
       <c r="E9" t="n">
-        <v>444.0</v>
+        <v>446.0</v>
       </c>
       <c r="F9" t="n">
         <v>31.0</v>
@@ -608,25 +602,25 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="n">
-        <v>109.0</v>
+        <v>22.0</v>
       </c>
       <c r="D10" t="n">
-        <v>43.0</v>
+        <v>8.0</v>
       </c>
       <c r="E10" t="n">
-        <v>22.0</v>
+        <v>5.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H10" t="n">
-        <v>21.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
@@ -634,25 +628,25 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="n">
-        <v>2.0</v>
+        <v>61759.0</v>
       </c>
       <c r="D11" t="n">
-        <v>2.0</v>
+        <v>1346.0</v>
       </c>
       <c r="E11" t="n">
-        <v>1.0</v>
+        <v>287.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1.0</v>
+        <v>30.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0</v>
+        <v>19.0</v>
       </c>
       <c r="H11" t="n">
-        <v>1.0</v>
+        <v>248.0</v>
       </c>
     </row>
     <row r="12">
@@ -660,25 +654,25 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="n">
-        <v>82.0</v>
+        <v>158652.0</v>
       </c>
       <c r="D12" t="n">
-        <v>55.0</v>
+        <v>1380.0</v>
       </c>
       <c r="E12" t="n">
-        <v>51.0</v>
+        <v>279.0</v>
       </c>
       <c r="F12" t="n">
-        <v>3.0</v>
+        <v>25.0</v>
       </c>
       <c r="G12" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="H12" t="n">
-        <v>44.0</v>
+        <v>233.0</v>
       </c>
     </row>
     <row r="13">
@@ -686,25 +680,25 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" t="n">
-        <v>61680.0</v>
+        <v>57431.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1343.0</v>
+        <v>1540.0</v>
       </c>
       <c r="E13" t="n">
-        <v>287.0</v>
+        <v>728.0</v>
       </c>
       <c r="F13" t="n">
-        <v>30.0</v>
+        <v>87.0</v>
       </c>
       <c r="G13" t="n">
-        <v>19.0</v>
+        <v>65.0</v>
       </c>
       <c r="H13" t="n">
-        <v>248.0</v>
+        <v>516.0</v>
       </c>
     </row>
     <row r="14">
@@ -712,25 +706,25 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="n">
-        <v>160465.0</v>
+        <v>2482.0</v>
       </c>
       <c r="D14" t="n">
-        <v>1382.0</v>
+        <v>195.0</v>
       </c>
       <c r="E14" t="n">
-        <v>279.0</v>
+        <v>45.0</v>
       </c>
       <c r="F14" t="n">
-        <v>25.0</v>
+        <v>12.0</v>
       </c>
       <c r="G14" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H14" t="n">
-        <v>233.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="15">
@@ -738,25 +732,25 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="n">
-        <v>57384.0</v>
+        <v>1398584.0</v>
       </c>
       <c r="D15" t="n">
-        <v>1524.0</v>
+        <v>12631.0</v>
       </c>
       <c r="E15" t="n">
-        <v>728.0</v>
+        <v>2872.0</v>
       </c>
       <c r="F15" t="n">
-        <v>86.0</v>
+        <v>221.0</v>
       </c>
       <c r="G15" t="n">
-        <v>65.0</v>
+        <v>91.0</v>
       </c>
       <c r="H15" t="n">
-        <v>516.0</v>
+        <v>2308.0</v>
       </c>
     </row>
     <row r="16">
@@ -764,25 +758,25 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="n">
-        <v>5.0</v>
+        <v>113.0</v>
       </c>
       <c r="D16" t="n">
-        <v>5.0</v>
+        <v>21.0</v>
       </c>
       <c r="E16" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="F16" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G16" t="n">
         <v>1.0</v>
       </c>
       <c r="H16" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="17">
@@ -790,25 +784,25 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" t="n">
-        <v>2482.0</v>
+        <v>2011.0</v>
       </c>
       <c r="D17" t="n">
-        <v>195.0</v>
+        <v>323.0</v>
       </c>
       <c r="E17" t="n">
-        <v>45.0</v>
+        <v>320.0</v>
       </c>
       <c r="F17" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G17" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="H17" t="n">
-        <v>38.0</v>
+        <v>292.0</v>
       </c>
     </row>
     <row r="18">
@@ -816,25 +810,25 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" t="n">
-        <v>1397461.0</v>
+        <v>37933.0</v>
       </c>
       <c r="D18" t="n">
-        <v>12655.0</v>
+        <v>256.0</v>
       </c>
       <c r="E18" t="n">
-        <v>2867.0</v>
+        <v>26.0</v>
       </c>
       <c r="F18" t="n">
-        <v>221.0</v>
+        <v>10.0</v>
       </c>
       <c r="G18" t="n">
-        <v>91.0</v>
+        <v>1.0</v>
       </c>
       <c r="H18" t="n">
-        <v>2307.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="19">
@@ -842,25 +836,25 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" t="n">
-        <v>113.0</v>
+        <v>16345.0</v>
       </c>
       <c r="D19" t="n">
-        <v>21.0</v>
+        <v>128.0</v>
       </c>
       <c r="E19" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="F19" t="n">
         <v>2.0</v>
       </c>
-      <c r="F19" t="n">
-        <v>4.0</v>
-      </c>
       <c r="G19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H19" t="n">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="20">
@@ -868,25 +862,25 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" t="n">
-        <v>2011.0</v>
+        <v>50.0</v>
       </c>
       <c r="D20" t="n">
-        <v>323.0</v>
+        <v>33.0</v>
       </c>
       <c r="E20" t="n">
-        <v>320.0</v>
+        <v>14.0</v>
       </c>
       <c r="F20" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="G20" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="H20" t="n">
-        <v>292.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="21">
@@ -894,25 +888,25 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" t="n">
-        <v>38724.0</v>
+        <v>24018.0</v>
       </c>
       <c r="D21" t="n">
-        <v>256.0</v>
+        <v>2264.0</v>
       </c>
       <c r="E21" t="n">
-        <v>26.0</v>
+        <v>1072.0</v>
       </c>
       <c r="F21" t="n">
-        <v>10.0</v>
+        <v>89.0</v>
       </c>
       <c r="G21" t="n">
-        <v>1.0</v>
+        <v>68.0</v>
       </c>
       <c r="H21" t="n">
-        <v>23.0</v>
+        <v>939.0</v>
       </c>
     </row>
     <row r="22">
@@ -920,25 +914,25 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" t="n">
-        <v>143.0</v>
+        <v>16130.0</v>
       </c>
       <c r="D22" t="n">
-        <v>81.0</v>
+        <v>1133.0</v>
       </c>
       <c r="E22" t="n">
-        <v>46.0</v>
+        <v>781.0</v>
       </c>
       <c r="F22" t="n">
-        <v>2.0</v>
+        <v>74.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1.0</v>
+        <v>55.0</v>
       </c>
       <c r="H22" t="n">
-        <v>45.0</v>
+        <v>521.0</v>
       </c>
     </row>
     <row r="23">
@@ -946,25 +940,25 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" t="n">
-        <v>16345.0</v>
+        <v>1340.0</v>
       </c>
       <c r="D23" t="n">
-        <v>128.0</v>
+        <v>116.0</v>
       </c>
       <c r="E23" t="n">
-        <v>19.0</v>
+        <v>92.0</v>
       </c>
       <c r="F23" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="G23" t="n">
         <v>2.0</v>
       </c>
       <c r="H23" t="n">
-        <v>18.0</v>
+        <v>89.0</v>
       </c>
     </row>
     <row r="24">
@@ -972,25 +966,25 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="n">
-        <v>38.0</v>
+        <v>673.0</v>
       </c>
       <c r="D24" t="n">
-        <v>26.0</v>
+        <v>359.0</v>
       </c>
       <c r="E24" t="n">
-        <v>13.0</v>
+        <v>218.0</v>
       </c>
       <c r="F24" t="n">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="G24" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="H24" t="n">
-        <v>13.0</v>
+        <v>174.0</v>
       </c>
     </row>
     <row r="25">
@@ -998,25 +992,25 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" t="n">
-        <v>27719.0</v>
+        <v>30860.0</v>
       </c>
       <c r="D25" t="n">
-        <v>2308.0</v>
+        <v>4561.0</v>
       </c>
       <c r="E25" t="n">
-        <v>1084.0</v>
+        <v>886.0</v>
       </c>
       <c r="F25" t="n">
-        <v>93.0</v>
+        <v>43.0</v>
       </c>
       <c r="G25" t="n">
-        <v>69.0</v>
+        <v>15.0</v>
       </c>
       <c r="H25" t="n">
-        <v>950.0</v>
+        <v>715.0</v>
       </c>
     </row>
     <row r="26">
@@ -1024,25 +1018,25 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" t="n">
-        <v>675.0</v>
+        <v>39603.0</v>
       </c>
       <c r="D26" t="n">
-        <v>361.0</v>
+        <v>1774.0</v>
       </c>
       <c r="E26" t="n">
-        <v>218.0</v>
+        <v>495.0</v>
       </c>
       <c r="F26" t="n">
-        <v>12.0</v>
+        <v>41.0</v>
       </c>
       <c r="G26" t="n">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
       <c r="H26" t="n">
-        <v>174.0</v>
+        <v>417.0</v>
       </c>
     </row>
     <row r="27">
@@ -1050,25 +1044,25 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" t="n">
-        <v>18029.0</v>
+        <v>88899.0</v>
       </c>
       <c r="D27" t="n">
-        <v>2911.0</v>
+        <v>646.0</v>
       </c>
       <c r="E27" t="n">
-        <v>638.0</v>
+        <v>95.0</v>
       </c>
       <c r="F27" t="n">
-        <v>35.0</v>
+        <v>14.0</v>
       </c>
       <c r="G27" t="n">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="H27" t="n">
-        <v>548.0</v>
+        <v>83.0</v>
       </c>
     </row>
     <row r="28">
@@ -1076,25 +1070,25 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" t="n">
-        <v>39487.0</v>
+        <v>8433.0</v>
       </c>
       <c r="D28" t="n">
-        <v>1774.0</v>
+        <v>397.0</v>
       </c>
       <c r="E28" t="n">
-        <v>495.0</v>
+        <v>274.0</v>
       </c>
       <c r="F28" t="n">
-        <v>41.0</v>
+        <v>49.0</v>
       </c>
       <c r="G28" t="n">
-        <v>13.0</v>
+        <v>38.0</v>
       </c>
       <c r="H28" t="n">
-        <v>417.0</v>
+        <v>218.0</v>
       </c>
     </row>
     <row r="29">
@@ -1102,25 +1096,25 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" t="n">
-        <v>93858.0</v>
+        <v>293.0</v>
       </c>
       <c r="D29" t="n">
-        <v>645.0</v>
+        <v>62.0</v>
       </c>
       <c r="E29" t="n">
-        <v>94.0</v>
+        <v>11.0</v>
       </c>
       <c r="F29" t="n">
-        <v>14.0</v>
+        <v>7.0</v>
       </c>
       <c r="G29" t="n">
         <v>1.0</v>
       </c>
       <c r="H29" t="n">
-        <v>83.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="30">
@@ -1128,25 +1122,25 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" t="n">
-        <v>8380.0</v>
+        <v>10966.0</v>
       </c>
       <c r="D30" t="n">
-        <v>397.0</v>
+        <v>1338.0</v>
       </c>
       <c r="E30" t="n">
-        <v>274.0</v>
+        <v>82.0</v>
       </c>
       <c r="F30" t="n">
-        <v>49.0</v>
+        <v>28.0</v>
       </c>
       <c r="G30" t="n">
-        <v>38.0</v>
+        <v>8.0</v>
       </c>
       <c r="H30" t="n">
-        <v>218.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="31">
@@ -1154,25 +1148,25 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" t="n">
-        <v>2.0</v>
+        <v>314137.0</v>
       </c>
       <c r="D31" t="n">
-        <v>1.0</v>
+        <v>3172.0</v>
       </c>
       <c r="E31" t="n">
-        <v>1.0</v>
+        <v>925.0</v>
       </c>
       <c r="F31" t="n">
-        <v>1.0</v>
+        <v>97.0</v>
       </c>
       <c r="G31" t="n">
-        <v>1.0</v>
+        <v>50.0</v>
       </c>
       <c r="H31" t="n">
-        <v>1.0</v>
+        <v>817.0</v>
       </c>
     </row>
     <row r="32">
@@ -1180,25 +1174,25 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" t="n">
-        <v>256.0</v>
+        <v>244.0</v>
       </c>
       <c r="D32" t="n">
-        <v>62.0</v>
+        <v>149.0</v>
       </c>
       <c r="E32" t="n">
-        <v>11.0</v>
+        <v>122.0</v>
       </c>
       <c r="F32" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G32" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H32" t="n">
-        <v>11.0</v>
+        <v>111.0</v>
       </c>
     </row>
     <row r="33">
@@ -1206,25 +1200,25 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C33" t="n">
-        <v>10829.0</v>
+        <v>280490.0</v>
       </c>
       <c r="D33" t="n">
-        <v>1334.0</v>
+        <v>1704.0</v>
       </c>
       <c r="E33" t="n">
-        <v>82.0</v>
+        <v>586.0</v>
       </c>
       <c r="F33" t="n">
-        <v>27.0</v>
+        <v>40.0</v>
       </c>
       <c r="G33" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="H33" t="n">
-        <v>72.0</v>
+        <v>459.0</v>
       </c>
     </row>
     <row r="34">
@@ -1232,25 +1226,25 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" t="n">
-        <v>301283.0</v>
+        <v>4471.0</v>
       </c>
       <c r="D34" t="n">
-        <v>3162.0</v>
+        <v>211.0</v>
       </c>
       <c r="E34" t="n">
-        <v>923.0</v>
+        <v>6.0</v>
       </c>
       <c r="F34" t="n">
-        <v>97.0</v>
+        <v>8.0</v>
       </c>
       <c r="G34" t="n">
-        <v>50.0</v>
+        <v>1.0</v>
       </c>
       <c r="H34" t="n">
-        <v>815.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="35">
@@ -1258,25 +1252,25 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" t="n">
-        <v>244.0</v>
+        <v>2555.0</v>
       </c>
       <c r="D35" t="n">
-        <v>149.0</v>
+        <v>490.0</v>
       </c>
       <c r="E35" t="n">
-        <v>122.0</v>
+        <v>364.0</v>
       </c>
       <c r="F35" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="G35" t="n">
         <v>5.0</v>
       </c>
       <c r="H35" t="n">
-        <v>111.0</v>
+        <v>319.0</v>
       </c>
     </row>
     <row r="36">
@@ -1284,25 +1278,25 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" t="n">
-        <v>280377.0</v>
+        <v>17909.0</v>
       </c>
       <c r="D36" t="n">
-        <v>1687.0</v>
+        <v>1827.0</v>
       </c>
       <c r="E36" t="n">
-        <v>586.0</v>
+        <v>1070.0</v>
       </c>
       <c r="F36" t="n">
-        <v>35.0</v>
+        <v>50.0</v>
       </c>
       <c r="G36" t="n">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="H36" t="n">
-        <v>459.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="37">
@@ -1310,25 +1304,25 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" t="n">
-        <v>2555.0</v>
+        <v>641.0</v>
       </c>
       <c r="D37" t="n">
-        <v>490.0</v>
+        <v>146.0</v>
       </c>
       <c r="E37" t="n">
-        <v>364.0</v>
+        <v>5.0</v>
       </c>
       <c r="F37" t="n">
         <v>9.0</v>
       </c>
       <c r="G37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H37" t="n">
         <v>5.0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>319.0</v>
       </c>
     </row>
     <row r="38">
@@ -1336,25 +1330,25 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" t="n">
-        <v>34.0</v>
+        <v>10171.0</v>
       </c>
       <c r="D38" t="n">
-        <v>34.0</v>
+        <v>1315.0</v>
       </c>
       <c r="E38" t="n">
-        <v>25.0</v>
+        <v>541.0</v>
       </c>
       <c r="F38" t="n">
-        <v>1.0</v>
+        <v>42.0</v>
       </c>
       <c r="G38" t="n">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
       <c r="H38" t="n">
-        <v>20.0</v>
+        <v>447.0</v>
       </c>
     </row>
     <row r="39">
@@ -1362,25 +1356,25 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" t="n">
-        <v>17395.0</v>
+        <v>291.0</v>
       </c>
       <c r="D39" t="n">
-        <v>1809.0</v>
+        <v>59.0</v>
       </c>
       <c r="E39" t="n">
-        <v>1062.0</v>
+        <v>58.0</v>
       </c>
       <c r="F39" t="n">
-        <v>49.0</v>
+        <v>2.0</v>
       </c>
       <c r="G39" t="n">
-        <v>15.0</v>
+        <v>1.0</v>
       </c>
       <c r="H39" t="n">
-        <v>896.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="40">
@@ -1388,25 +1382,25 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" t="n">
-        <v>146.0</v>
+        <v>2404.0</v>
       </c>
       <c r="D40" t="n">
-        <v>65.0</v>
+        <v>160.0</v>
       </c>
       <c r="E40" t="n">
-        <v>2.0</v>
+        <v>110.0</v>
       </c>
       <c r="F40" t="n">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
       <c r="G40" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="H40" t="n">
-        <v>2.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="41">
@@ -1414,25 +1408,25 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" t="n">
-        <v>11190.0</v>
+        <v>4247.0</v>
       </c>
       <c r="D41" t="n">
-        <v>1398.0</v>
+        <v>592.0</v>
       </c>
       <c r="E41" t="n">
-        <v>550.0</v>
+        <v>119.0</v>
       </c>
       <c r="F41" t="n">
-        <v>43.0</v>
+        <v>20.0</v>
       </c>
       <c r="G41" t="n">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="H41" t="n">
-        <v>454.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="42">
@@ -1440,25 +1434,25 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" t="n">
-        <v>291.0</v>
+        <v>7669.0</v>
       </c>
       <c r="D42" t="n">
-        <v>59.0</v>
+        <v>394.0</v>
       </c>
       <c r="E42" t="n">
-        <v>58.0</v>
+        <v>30.0</v>
       </c>
       <c r="F42" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="G42" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H42" t="n">
-        <v>52.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="43">
@@ -1466,25 +1460,25 @@
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" t="n">
-        <v>1186.0</v>
+        <v>7.0</v>
       </c>
       <c r="D43" t="n">
-        <v>343.0</v>
+        <v>3.0</v>
       </c>
       <c r="E43" t="n">
-        <v>81.0</v>
+        <v>1.0</v>
       </c>
       <c r="F43" t="n">
-        <v>20.0</v>
+        <v>3.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H43" t="n">
-        <v>71.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
@@ -1492,25 +1486,25 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="n">
-        <v>4184.0</v>
+        <v>367761.0</v>
       </c>
       <c r="D44" t="n">
-        <v>232.0</v>
+        <v>739.0</v>
       </c>
       <c r="E44" t="n">
-        <v>21.0</v>
+        <v>100.0</v>
       </c>
       <c r="F44" t="n">
-        <v>9.0</v>
+        <v>17.0</v>
       </c>
       <c r="G44" t="n">
-        <v>3.0</v>
+        <v>11.0</v>
       </c>
       <c r="H44" t="n">
-        <v>20.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="45">
@@ -1518,25 +1512,25 @@
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" t="n">
-        <v>5.0</v>
+        <v>165.0</v>
       </c>
       <c r="D45" t="n">
-        <v>2.0</v>
+        <v>31.0</v>
       </c>
       <c r="E45" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="F45" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="G45" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H45" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="46">
@@ -1544,25 +1538,25 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" t="n">
-        <v>367775.0</v>
+        <v>3.0</v>
       </c>
       <c r="D46" t="n">
-        <v>747.0</v>
+        <v>2.0</v>
       </c>
       <c r="E46" t="n">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="F46" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
       <c r="G46" t="n">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="H46" t="n">
-        <v>97.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="47">
@@ -1570,25 +1564,25 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" t="n">
-        <v>165.0</v>
+        <v>16.0</v>
       </c>
       <c r="D47" t="n">
-        <v>31.0</v>
+        <v>8.0</v>
       </c>
       <c r="E47" t="n">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="F47" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="G47" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H47" t="n">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="48">
@@ -1596,51 +1590,25 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" t="n">
-        <v>171.0</v>
+        <v>1034.0</v>
       </c>
       <c r="D48" t="n">
-        <v>33.0</v>
+        <v>137.0</v>
       </c>
       <c r="E48" t="n">
-        <v>2.0</v>
+        <v>128.0</v>
       </c>
       <c r="F48" t="n">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="G48" t="n">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="H48" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D49" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H49" t="n">
-        <v>2.0</v>
+        <v>105.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>